<commit_message>
chore: sync empty local database with new schema columns
</commit_message>
<xml_diff>
--- a/flux_financial_database.xlsx
+++ b/flux_financial_database.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,92 +466,6 @@
       <c r="I1" t="inlineStr">
         <is>
           <t>CreatedAt</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AC1001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>jeevan</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>123456</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>jeevan babu kb</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>kbjeevanbabu803@gmail.com</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>9342977191</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2026-02-14 18:07:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AC1002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>suraj</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>234567</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>suraj</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>surajarjun475@gmail.com</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>8861254291</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2026-02-16 12:31:27</t>
         </is>
       </c>
     </row>
@@ -566,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -592,246 +506,57 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>SessionDuration</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>TransactionAmount</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>CyberRiskScore</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>TransactionType</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>SessionID</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>LoginHour</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>SessionDuration</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>PagesVisited</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ClickRate</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>NewDeviceLogin</t>
-        </is>
-      </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>NewLocationLogin</t>
+          <t>LargeTransaction</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>TransactionAmount</t>
+          <t>DeviceTrustScore</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>LargeTransaction</t>
+          <t>RapidTransactions</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>RapidTransactions</t>
+          <t>FailedLoginCount</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>BeneficiaryAdded</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>FailedLoginCount</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
           <t>PasswordChanged</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>DeviceTrustScore</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>ImpossibleTravel</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>CyberRiskScore</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>TransactionType</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>LOG-1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AC1001</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2026-02-14 20:21:17</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>SES-DEPOSIT</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>10</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Credit</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Deposit via Bank Transfer</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LOG-2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AC1001</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2026-02-16 12:17:37</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>SES-DEPOSIT</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>10</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Credit</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Deposit via Bank Transfer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fill all 21 ActivityLogs columns including LoginHour, RiskLabel, Channel and ML fields
</commit_message>
<xml_diff>
--- a/flux_financial_database.xlsx
+++ b/flux_financial_database.xlsx
@@ -480,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,57 +506,92 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>TransactionType</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>SessionID</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>TransactionAmount</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>SessionDuration</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>TransactionAmount</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>LoginHour</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>FailedLoginCount</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>NewDeviceLogin</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>PasswordChanged</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Channel</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>PagesVisited</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>ClickRate</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>RapidTransactions</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>BeneficiaryAdded</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>LargeTransaction</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>DeviceTrustScore</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
         <is>
           <t>CyberRiskScore</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>TransactionType</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>SessionID</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>LargeTransaction</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>DeviceTrustScore</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>RapidTransactions</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>FailedLoginCount</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>PasswordChanged</t>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>RiskLabel</t>
         </is>
       </c>
     </row>

</xml_diff>